<commit_message>
updated syntax to rename column; changed modified files' folder names
</commit_message>
<xml_diff>
--- a/main_census_merge/reference_data_files/Census_Variables_Mapping.xlsx
+++ b/main_census_merge/reference_data_files/Census_Variables_Mapping.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sshaik2\Criminal_Justice\Projects\main_census_merge\reference_data_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sshaik2\PycharmProjects\projects\research-projects\main_census_merge\reference_data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000"/>
   </bookViews>
   <sheets>
     <sheet name="Cities-2000" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="566">
   <si>
     <t>GEO.id</t>
   </si>
@@ -1854,6 +1854,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1861,12 +1867,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2150,8 +2150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69:XFD69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2185,32 +2185,32 @@
       <c r="I1" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="19" t="s">
         <v>307</v>
       </c>
-      <c r="K1" s="17"/>
-      <c r="L1" s="18" t="s">
+      <c r="K1" s="19"/>
+      <c r="L1" s="20" t="s">
         <v>333</v>
       </c>
-      <c r="M1" s="18"/>
+      <c r="M1" s="20"/>
     </row>
     <row r="2" spans="1:13" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>326</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="17" t="s">
         <v>540</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="17" t="s">
         <v>541</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="17" t="s">
         <v>544</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="17" t="s">
         <v>542</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="17" t="s">
         <v>543</v>
       </c>
       <c r="G2" s="10"/>
@@ -2438,7 +2438,7 @@
       <c r="K10" t="s">
         <v>305</v>
       </c>
-      <c r="L10" s="21" t="s">
+      <c r="L10" s="18" t="s">
         <v>561</v>
       </c>
     </row>
@@ -2473,7 +2473,7 @@
       <c r="K11" t="s">
         <v>306</v>
       </c>
-      <c r="L11" s="21" t="s">
+      <c r="L11" s="18" t="s">
         <v>562</v>
       </c>
     </row>
@@ -2508,7 +2508,7 @@
       <c r="K12" s="11" t="s">
         <v>308</v>
       </c>
-      <c r="L12" s="21" t="s">
+      <c r="L12" s="18" t="s">
         <v>563</v>
       </c>
     </row>
@@ -2543,7 +2543,7 @@
       <c r="K13" s="11" t="s">
         <v>309</v>
       </c>
-      <c r="L13" s="21" t="s">
+      <c r="L13" s="18" t="s">
         <v>564</v>
       </c>
     </row>
@@ -2613,7 +2613,7 @@
       <c r="K15" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="L15" s="21" t="s">
+      <c r="L15" s="18" t="s">
         <v>547</v>
       </c>
     </row>
@@ -2683,7 +2683,7 @@
       <c r="K17" s="11" t="s">
         <v>313</v>
       </c>
-      <c r="L17" s="21" t="s">
+      <c r="L17" s="18" t="s">
         <v>548</v>
       </c>
     </row>
@@ -2753,7 +2753,7 @@
       <c r="K19" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="L19" s="21" t="s">
+      <c r="L19" s="18" t="s">
         <v>550</v>
       </c>
     </row>
@@ -2823,7 +2823,7 @@
       <c r="K21" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="L21" s="21" t="s">
+      <c r="L21" s="18" t="s">
         <v>552</v>
       </c>
     </row>
@@ -2858,7 +2858,7 @@
       <c r="K22" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="L22" s="21" t="s">
+      <c r="L22" s="18" t="s">
         <v>553</v>
       </c>
     </row>
@@ -2963,7 +2963,7 @@
       <c r="K25" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="L25" s="21" t="s">
+      <c r="L25" s="18" t="s">
         <v>556</v>
       </c>
     </row>
@@ -2998,7 +2998,7 @@
       <c r="K26" s="11" t="s">
         <v>322</v>
       </c>
-      <c r="L26" s="21" t="s">
+      <c r="L26" s="18" t="s">
         <v>557</v>
       </c>
     </row>
@@ -3103,7 +3103,7 @@
       <c r="K29" s="11" t="s">
         <v>325</v>
       </c>
-      <c r="L29" s="21" t="s">
+      <c r="L29" s="18" t="s">
         <v>560</v>
       </c>
     </row>
@@ -3718,12 +3718,8 @@
       </c>
     </row>
     <row r="69" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I69" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="L69" s="16">
-        <v>2000</v>
-      </c>
+      <c r="I69" s="4"/>
+      <c r="L69" s="16"/>
       <c r="M69" s="13"/>
     </row>
   </sheetData>
@@ -3757,10 +3753,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="19">
+      <c r="A1" s="21">
         <v>2010</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="21"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -3778,14 +3774,14 @@
       <c r="D3" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="19" t="s">
         <v>307</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="18" t="s">
+      <c r="F3" s="19"/>
+      <c r="G3" s="20" t="s">
         <v>334</v>
       </c>
-      <c r="H3" s="18"/>
+      <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -4698,7 +4694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated new census variables' mapping
</commit_message>
<xml_diff>
--- a/main_census_merge/reference_data_files/Census_Variables_Mapping.xlsx
+++ b/main_census_merge/reference_data_files/Census_Variables_Mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sshaik2\PycharmProjects\projects\research-projects\main_census_merge\reference_data_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sshaik2\Criminal_Justice\Projects\main_census_merge\reference_data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1626" uniqueCount="584">
   <si>
     <t>GEO.id</t>
   </si>
@@ -1652,15 +1652,9 @@
     <t>P012 (Total pop - Sex By Age)</t>
   </si>
   <si>
-    <t>P012A(White alone-sex by age)</t>
-  </si>
-  <si>
     <t>P012H(Hispanic or Latino-sex by age)</t>
   </si>
   <si>
-    <t>P012I(White alone, not Hispanic or Latino</t>
-  </si>
-  <si>
     <t>P012B(Black or African American alone-sex by age)</t>
   </si>
   <si>
@@ -1670,68 +1664,128 @@
     <t>sum(P012AVD30-P012AVD34)</t>
   </si>
   <si>
-    <t>sum(P012AVD03-P012AVD25). Is this same as P012AVD02 (Male:)?</t>
-  </si>
-  <si>
-    <t>sum(P012AVD27-P012AVD49). Is this same as P012AVD26(Female:)?</t>
-  </si>
-  <si>
     <t>sum(P012BVD06-P012BVD10)</t>
   </si>
   <si>
-    <t>sum(P012BVD03-P012BVD25). Is this same as P012BVD02 (Male:)?</t>
-  </si>
-  <si>
     <t>sum(P012BVD30-P012BVD34)</t>
   </si>
   <si>
-    <t>sum(P012BVD27-P012BVD49). Is this same as P012BVD26(Female:)?</t>
-  </si>
-  <si>
-    <t>sum(P012HVD03-P012HVD25). Is this same as P012HVD02 (Male:)?</t>
-  </si>
-  <si>
     <t>sum(P012HVD06-P012HVD10)</t>
   </si>
   <si>
     <t>sum(P012HVD30-P012HVD34)</t>
   </si>
   <si>
-    <t>sum(P012HVD27-P012HVD49). Is this same as P012HVD26(Female:)?</t>
-  </si>
-  <si>
-    <t>sum(P012IVD03-P012IVD25). Is this same as P012IVD02 (Male:)?</t>
-  </si>
-  <si>
     <t>sum(P012IVD06-P012IVD10)</t>
   </si>
   <si>
     <t>sum(P012IVD30-P012IVD34)</t>
   </si>
   <si>
-    <t>sum(P012IVD27-P012IVD49). Is this same as P012IVD26(Female:)?</t>
-  </si>
-  <si>
-    <t>P012AVD01 (Male:+Female:)?</t>
-  </si>
-  <si>
-    <t>P012BVD01 (Male:+Female:)?</t>
-  </si>
-  <si>
-    <t>P012IVD01 (Male:+Female:)?</t>
-  </si>
-  <si>
-    <t>P012HVD01 (Male:+Female:)?</t>
-  </si>
-  <si>
-    <t>P012VD01(Total: - Total pop)</t>
+    <t>P012I(White alone, not Hispanic or Latino - sex by age) Ethnicity</t>
+  </si>
+  <si>
+    <t>P012A(White alone-sex by age) Race</t>
+  </si>
+  <si>
+    <t>P012AVD01 (Male:+Female:)</t>
+  </si>
+  <si>
+    <t>P012BVD01 (Male:+Female:)</t>
+  </si>
+  <si>
+    <t>P012IVD01 (Male:+Female:)</t>
+  </si>
+  <si>
+    <t>P012HVD01 (Male:+Female:)</t>
+  </si>
+  <si>
+    <t>sum(P012BVD03-P012BVD25). Is this same as P012BVD02 (Male:)</t>
+  </si>
+  <si>
+    <t>sum(P012BVD27-P012BVD49). Is this same as P012BVD26(Female:)</t>
+  </si>
+  <si>
+    <t>sum(P012HVD03-P012HVD25). Is this same as P012HVD02 (Male:)</t>
+  </si>
+  <si>
+    <t>sum(P012HVD27-P012HVD49). Is this same as P012HVD26(Female:)</t>
+  </si>
+  <si>
+    <t>sum(P012IVD03-P012IVD25). Is this same as P012IVD02 (Male:)</t>
+  </si>
+  <si>
+    <t>sum(P012IVD27-P012IVD49). Is this same as P012IVD26(Female:)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P12AD001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">P12BD001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">P12HD001 </t>
+  </si>
+  <si>
+    <t>sum(P12AD006-P12AD010)</t>
+  </si>
+  <si>
+    <t>sum(P012AVD03-P012AVD25). same as P012AVD02 (Male:)</t>
+  </si>
+  <si>
+    <t>sum(P12AD003-P12AD025). same as P12AD002 (Male:)</t>
+  </si>
+  <si>
+    <t>sum(P12AD030-P12AD034)</t>
+  </si>
+  <si>
+    <t>sum(P12BD006-P12BD010)</t>
+  </si>
+  <si>
+    <t>sum(P12BD030-P12BD034)</t>
+  </si>
+  <si>
+    <t>sum(P012AVD27-P012AVD49).same as P012AVD26(Female:)</t>
+  </si>
+  <si>
+    <t>sum(P12AD027-P12AD049).same as P12AD026(Female:)</t>
+  </si>
+  <si>
+    <t>sum(P12BD003-P12BD025). Is this same as P12BD002 (Male:)</t>
+  </si>
+  <si>
+    <t>sum(P12BD027-P12BD049). Is this same as P12BD026(Female:)</t>
+  </si>
+  <si>
+    <t>sum(P12HD003-P12HD025). Is this same as P12HD002 (Male:)</t>
+  </si>
+  <si>
+    <t>sum(P12HD006-P12HD010)</t>
+  </si>
+  <si>
+    <t>sum(P12HD030-P12HD034)</t>
+  </si>
+  <si>
+    <t>sum(P12HD027-P12HD049). Is this same as P12HD026(Female:)</t>
+  </si>
+  <si>
+    <t>sum(P12ID003-P12ID025). Is this same as P12ID002 (Male:)</t>
+  </si>
+  <si>
+    <t>sum(P12ID006-P12ID010)</t>
+  </si>
+  <si>
+    <t>sum(P12ID030-P12ID034)</t>
+  </si>
+  <si>
+    <t>sum(P12ID027-P12ID049). Is this same as P12ID026(Female:)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1782,6 +1836,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1821,7 +1890,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1843,7 +1912,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1868,6 +1936,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2150,8 +2232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69:XFD69"/>
+    <sheetView tabSelected="1" topLeftCell="H24" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2163,8 +2245,8 @@
     <col min="9" max="9" width="21.28515625" customWidth="1"/>
     <col min="10" max="10" width="25.140625" customWidth="1"/>
     <col min="11" max="11" width="24.5703125" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" style="11" customWidth="1"/>
-    <col min="13" max="13" width="19.85546875" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" style="24" customWidth="1"/>
+    <col min="13" max="13" width="19.85546875" style="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2178,48 +2260,50 @@
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
       <c r="F1" s="12"/>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="H1" s="14"/>
+      <c r="H1" s="13"/>
       <c r="I1" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="18" t="s">
         <v>307</v>
       </c>
-      <c r="K1" s="19"/>
-      <c r="L1" s="20" t="s">
+      <c r="K1" s="18"/>
+      <c r="L1" s="22" t="s">
         <v>333</v>
       </c>
-      <c r="M1" s="20"/>
+      <c r="M1" s="22" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="2" spans="1:13" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>326</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>540</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
+        <v>552</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>542</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>541</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>544</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>542</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>543</v>
+      <c r="F2" s="16" t="s">
+        <v>551</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="6"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="25"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2246,7 +2330,7 @@
       <c r="I3" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="24" t="s">
         <v>328</v>
       </c>
     </row>
@@ -2275,12 +2359,12 @@
       <c r="I4" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="24" t="s">
         <v>329</v>
       </c>
-      <c r="M4" s="11"/>
-    </row>
-    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="M4" s="24"/>
+    </row>
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -2305,7 +2389,7 @@
       <c r="I5" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="L5" s="24" t="s">
         <v>330</v>
       </c>
     </row>
@@ -2334,7 +2418,7 @@
       <c r="I6" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="24" t="s">
         <v>331</v>
       </c>
     </row>
@@ -2363,21 +2447,23 @@
       <c r="I7" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="L7" s="11" t="s">
+      <c r="L7" s="24" t="s">
         <v>332</v>
       </c>
-      <c r="M7" s="11"/>
+      <c r="M7" s="24"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I8" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="24">
         <v>2000</v>
       </c>
-      <c r="M8" s="11"/>
-    </row>
-    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="M8" s="24">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -2402,10 +2488,12 @@
       <c r="I9" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="L9" s="16" t="s">
-        <v>565</v>
-      </c>
-      <c r="M9" s="13"/>
+      <c r="L9" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="M9" s="24" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -2438,8 +2526,11 @@
       <c r="K10" t="s">
         <v>305</v>
       </c>
-      <c r="L10" s="18" t="s">
-        <v>561</v>
+      <c r="L10" s="24" t="s">
+        <v>553</v>
+      </c>
+      <c r="M10" s="26" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -2473,44 +2564,48 @@
       <c r="K11" t="s">
         <v>306</v>
       </c>
-      <c r="L11" s="18" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="L11" s="24" t="s">
+        <v>554</v>
+      </c>
+      <c r="M11" s="26" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="10" t="s">
         <v>349</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="10" t="s">
         <v>398</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="10" t="s">
         <v>447</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="10" t="s">
         <v>496</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="J12" s="11" t="s">
+      <c r="J12" s="17" t="s">
         <v>286</v>
       </c>
-      <c r="K12" s="11" t="s">
+      <c r="K12" s="17" t="s">
         <v>308</v>
       </c>
-      <c r="L12" s="18" t="s">
-        <v>563</v>
-      </c>
+      <c r="L12" s="24" t="s">
+        <v>555</v>
+      </c>
+      <c r="M12" s="26"/>
     </row>
     <row r="13" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -2543,8 +2638,11 @@
       <c r="K13" s="11" t="s">
         <v>309</v>
       </c>
-      <c r="L13" s="18" t="s">
-        <v>564</v>
+      <c r="L13" s="24" t="s">
+        <v>556</v>
+      </c>
+      <c r="M13" s="26" t="s">
+        <v>565</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -2578,11 +2676,14 @@
       <c r="K14" s="11" t="s">
         <v>310</v>
       </c>
-      <c r="L14" s="11" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="L14" s="24" t="s">
+        <v>543</v>
+      </c>
+      <c r="M14" s="24" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -2613,8 +2714,11 @@
       <c r="K15" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="L15" s="18" t="s">
-        <v>547</v>
+      <c r="L15" s="24" t="s">
+        <v>567</v>
+      </c>
+      <c r="M15" s="24" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -2648,11 +2752,14 @@
       <c r="K16" s="11" t="s">
         <v>312</v>
       </c>
-      <c r="L16" s="11" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="L16" s="24" t="s">
+        <v>544</v>
+      </c>
+      <c r="M16" s="24" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -2683,11 +2790,14 @@
       <c r="K17" s="11" t="s">
         <v>313</v>
       </c>
-      <c r="L17" s="18" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="L17" s="24" t="s">
+        <v>572</v>
+      </c>
+      <c r="M17" s="24" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -2718,11 +2828,14 @@
       <c r="K18" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="L18" s="11" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="L18" s="24" t="s">
+        <v>545</v>
+      </c>
+      <c r="M18" s="24" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2753,11 +2866,14 @@
       <c r="K19" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="L19" s="18" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="L19" s="24" t="s">
+        <v>557</v>
+      </c>
+      <c r="M19" s="24" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2788,11 +2904,14 @@
       <c r="K20" s="11" t="s">
         <v>317</v>
       </c>
-      <c r="L20" s="11" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="L20" s="24" t="s">
+        <v>546</v>
+      </c>
+      <c r="M20" s="24" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -2823,11 +2942,14 @@
       <c r="K21" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="L21" s="18" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="L21" s="24" t="s">
+        <v>558</v>
+      </c>
+      <c r="M21" s="24" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -2858,11 +2980,14 @@
       <c r="K22" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="L22" s="18" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="L22" s="24" t="s">
+        <v>559</v>
+      </c>
+      <c r="M22" s="24" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2893,11 +3018,14 @@
       <c r="K23" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="L23" s="11" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="L23" s="24" t="s">
+        <v>547</v>
+      </c>
+      <c r="M23" s="24" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -2928,11 +3056,14 @@
       <c r="K24" s="11" t="s">
         <v>320</v>
       </c>
-      <c r="L24" s="11" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="L24" s="24" t="s">
+        <v>548</v>
+      </c>
+      <c r="M24" s="24" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -2963,46 +3094,52 @@
       <c r="K25" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="L25" s="18" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="L25" s="24" t="s">
+        <v>560</v>
+      </c>
+      <c r="M25" s="24" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="10" t="s">
         <v>363</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="10" t="s">
         <v>412</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="10" t="s">
         <v>461</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="10" t="s">
         <v>510</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="I26" s="4" t="s">
+      <c r="I26" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="J26" s="11" t="s">
+      <c r="J26" s="17" t="s">
         <v>299</v>
       </c>
-      <c r="K26" s="11" t="s">
+      <c r="K26" s="17" t="s">
         <v>322</v>
       </c>
-      <c r="L26" s="18" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="L26" s="24" t="s">
+        <v>561</v>
+      </c>
+      <c r="M26" s="24" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -3033,11 +3170,14 @@
       <c r="K27" s="11" t="s">
         <v>323</v>
       </c>
-      <c r="L27" s="11" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="L27" s="24" t="s">
+        <v>549</v>
+      </c>
+      <c r="M27" s="24" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -3068,46 +3208,52 @@
       <c r="K28" s="11" t="s">
         <v>324</v>
       </c>
-      <c r="L28" s="11" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="L28" s="24" t="s">
+        <v>550</v>
+      </c>
+      <c r="M28" s="24" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="10" t="s">
         <v>415</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="10" t="s">
         <v>464</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="10" t="s">
         <v>513</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="I29" s="4" t="s">
+      <c r="I29" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="J29" s="11" t="s">
+      <c r="J29" s="17" t="s">
         <v>302</v>
       </c>
-      <c r="K29" s="11" t="s">
+      <c r="K29" s="17" t="s">
         <v>325</v>
       </c>
-      <c r="L29" s="18" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="L29" s="24" t="s">
+        <v>562</v>
+      </c>
+      <c r="M29" s="24" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -3136,7 +3282,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -3165,7 +3311,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -3717,15 +3863,12 @@
         <v>342</v>
       </c>
     </row>
-    <row r="69" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I69" s="4"/>
-      <c r="L69" s="16"/>
-      <c r="M69" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3737,7 +3880,7 @@
   <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3753,10 +3896,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="21">
+      <c r="A1" s="20">
         <v>2010</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="20"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -3768,20 +3911,20 @@
       <c r="B3" s="12" t="s">
         <v>340</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>282</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="18" t="s">
         <v>307</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="20" t="s">
+      <c r="F3" s="18"/>
+      <c r="G3" s="19" t="s">
         <v>334</v>
       </c>
-      <c r="H3" s="20"/>
+      <c r="H3" s="19"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -3794,7 +3937,7 @@
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="15"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3895,7 +4038,7 @@
       <c r="D10" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="15" t="s">
         <v>231</v>
       </c>
       <c r="H10" t="s">
@@ -3906,7 +4049,7 @@
       <c r="D11" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="15">
         <v>2010</v>
       </c>
     </row>
@@ -4682,7 +4825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
added code to generate new census variables; need to resolve issue with (r...
</commit_message>
<xml_diff>
--- a/main_census_merge/reference_data_files/Census_Variables_Mapping.xlsx
+++ b/main_census_merge/reference_data_files/Census_Variables_Mapping.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1626" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="589">
   <si>
     <t>GEO.id</t>
   </si>
@@ -1779,6 +1779,21 @@
   </si>
   <si>
     <t>sum(P12ID027-P12ID049). Is this same as P12ID026(Female:)</t>
+  </si>
+  <si>
+    <t>7th column or 6th index</t>
+  </si>
+  <si>
+    <t>12th -  16th cols or 11th-16th indices</t>
+  </si>
+  <si>
+    <t>8th col or 7th index</t>
+  </si>
+  <si>
+    <t>36th-40th cols or 35th-40th indices</t>
+  </si>
+  <si>
+    <t>32nd col or 31st index</t>
   </si>
 </sst>
 </file>
@@ -1927,15 +1942,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1950,6 +1956,15 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2230,10 +2245,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M69"/>
+  <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H24" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView tabSelected="1" topLeftCell="I23" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2245,11 +2260,12 @@
     <col min="9" max="9" width="21.28515625" customWidth="1"/>
     <col min="10" max="10" width="25.140625" customWidth="1"/>
     <col min="11" max="11" width="24.5703125" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" style="24" customWidth="1"/>
-    <col min="13" max="13" width="19.85546875" style="26" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" style="21" customWidth="1"/>
+    <col min="13" max="13" width="19.85546875" style="23" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>281</v>
       </c>
@@ -2267,18 +2283,18 @@
       <c r="I1" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="24" t="s">
         <v>307</v>
       </c>
-      <c r="K1" s="18"/>
-      <c r="L1" s="22" t="s">
+      <c r="K1" s="24"/>
+      <c r="L1" s="19" t="s">
         <v>333</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="M1" s="19" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>326</v>
       </c>
@@ -2302,10 +2318,10 @@
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="25"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L2" s="20"/>
+      <c r="M2" s="22"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2330,11 +2346,11 @@
       <c r="I3" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="L3" s="24" t="s">
+      <c r="L3" s="21" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -2359,12 +2375,12 @@
       <c r="I4" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="L4" s="21" t="s">
         <v>329</v>
       </c>
-      <c r="M4" s="24"/>
-    </row>
-    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="M4" s="21"/>
+    </row>
+    <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -2389,11 +2405,11 @@
       <c r="I5" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="L5" s="24" t="s">
+      <c r="L5" s="21" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2418,11 +2434,11 @@
       <c r="I6" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="L6" s="24" t="s">
+      <c r="L6" s="21" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2447,23 +2463,23 @@
       <c r="I7" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="L7" s="24" t="s">
+      <c r="L7" s="21" t="s">
         <v>332</v>
       </c>
-      <c r="M7" s="24"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M7" s="21"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I8" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="L8" s="24">
+      <c r="L8" s="21">
         <v>2000</v>
       </c>
-      <c r="M8" s="24">
+      <c r="M8" s="21">
         <v>2010</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -2488,14 +2504,17 @@
       <c r="I9" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="L9" s="24" t="s">
+      <c r="L9" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="M9" s="24" t="s">
+      <c r="M9" s="21" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N9" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -2526,14 +2545,17 @@
       <c r="K10" t="s">
         <v>305</v>
       </c>
-      <c r="L10" s="24" t="s">
+      <c r="L10" s="21" t="s">
         <v>553</v>
       </c>
-      <c r="M10" s="26" t="s">
+      <c r="M10" s="23" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N10" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -2564,14 +2586,17 @@
       <c r="K11" t="s">
         <v>306</v>
       </c>
-      <c r="L11" s="24" t="s">
+      <c r="L11" s="21" t="s">
         <v>554</v>
       </c>
-      <c r="M11" s="26" t="s">
+      <c r="M11" s="23" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="N11" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>8</v>
       </c>
@@ -2593,7 +2618,7 @@
       <c r="G12" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="I12" s="21" t="s">
+      <c r="I12" s="18" t="s">
         <v>162</v>
       </c>
       <c r="J12" s="17" t="s">
@@ -2602,12 +2627,12 @@
       <c r="K12" s="17" t="s">
         <v>308</v>
       </c>
-      <c r="L12" s="24" t="s">
+      <c r="L12" s="21" t="s">
         <v>555</v>
       </c>
-      <c r="M12" s="26"/>
-    </row>
-    <row r="13" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="M12" s="23"/>
+    </row>
+    <row r="13" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -2638,14 +2663,17 @@
       <c r="K13" s="11" t="s">
         <v>309</v>
       </c>
-      <c r="L13" s="24" t="s">
+      <c r="L13" s="21" t="s">
         <v>556</v>
       </c>
-      <c r="M13" s="26" t="s">
+      <c r="M13" s="23" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="N13" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -2676,14 +2704,17 @@
       <c r="K14" s="11" t="s">
         <v>310</v>
       </c>
-      <c r="L14" s="24" t="s">
+      <c r="L14" s="21" t="s">
         <v>543</v>
       </c>
-      <c r="M14" s="24" t="s">
+      <c r="M14" s="21" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="N14" s="11" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -2714,14 +2745,17 @@
       <c r="K15" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="L15" s="24" t="s">
+      <c r="L15" s="21" t="s">
         <v>567</v>
       </c>
-      <c r="M15" s="24" t="s">
+      <c r="M15" s="21" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N15" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -2752,14 +2786,17 @@
       <c r="K16" s="11" t="s">
         <v>312</v>
       </c>
-      <c r="L16" s="24" t="s">
+      <c r="L16" s="21" t="s">
         <v>544</v>
       </c>
-      <c r="M16" s="24" t="s">
+      <c r="M16" s="21" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="N16" s="11" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -2790,14 +2827,17 @@
       <c r="K17" s="11" t="s">
         <v>313</v>
       </c>
-      <c r="L17" s="24" t="s">
+      <c r="L17" s="21" t="s">
         <v>572</v>
       </c>
-      <c r="M17" s="24" t="s">
+      <c r="M17" s="21" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N17" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -2828,14 +2868,14 @@
       <c r="K18" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="L18" s="24" t="s">
+      <c r="L18" s="21" t="s">
         <v>545</v>
       </c>
-      <c r="M18" s="24" t="s">
+      <c r="M18" s="21" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2866,14 +2906,14 @@
       <c r="K19" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="L19" s="24" t="s">
+      <c r="L19" s="21" t="s">
         <v>557</v>
       </c>
-      <c r="M19" s="24" t="s">
+      <c r="M19" s="21" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2904,14 +2944,14 @@
       <c r="K20" s="11" t="s">
         <v>317</v>
       </c>
-      <c r="L20" s="24" t="s">
+      <c r="L20" s="21" t="s">
         <v>546</v>
       </c>
-      <c r="M20" s="24" t="s">
+      <c r="M20" s="21" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -2942,14 +2982,14 @@
       <c r="K21" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="L21" s="24" t="s">
+      <c r="L21" s="21" t="s">
         <v>558</v>
       </c>
-      <c r="M21" s="24" t="s">
+      <c r="M21" s="21" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -2980,14 +3020,14 @@
       <c r="K22" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="L22" s="24" t="s">
+      <c r="L22" s="21" t="s">
         <v>559</v>
       </c>
-      <c r="M22" s="24" t="s">
+      <c r="M22" s="21" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -3018,14 +3058,14 @@
       <c r="K23" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="L23" s="24" t="s">
+      <c r="L23" s="21" t="s">
         <v>547</v>
       </c>
-      <c r="M23" s="24" t="s">
+      <c r="M23" s="21" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -3056,14 +3096,14 @@
       <c r="K24" s="11" t="s">
         <v>320</v>
       </c>
-      <c r="L24" s="24" t="s">
+      <c r="L24" s="21" t="s">
         <v>548</v>
       </c>
-      <c r="M24" s="24" t="s">
+      <c r="M24" s="21" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -3094,14 +3134,14 @@
       <c r="K25" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="L25" s="24" t="s">
+      <c r="L25" s="21" t="s">
         <v>560</v>
       </c>
-      <c r="M25" s="24" t="s">
+      <c r="M25" s="21" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>22</v>
       </c>
@@ -3123,7 +3163,7 @@
       <c r="G26" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="I26" s="21" t="s">
+      <c r="I26" s="18" t="s">
         <v>176</v>
       </c>
       <c r="J26" s="17" t="s">
@@ -3132,14 +3172,14 @@
       <c r="K26" s="17" t="s">
         <v>322</v>
       </c>
-      <c r="L26" s="24" t="s">
+      <c r="L26" s="21" t="s">
         <v>561</v>
       </c>
-      <c r="M26" s="24" t="s">
+      <c r="M26" s="21" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -3170,14 +3210,14 @@
       <c r="K27" s="11" t="s">
         <v>323</v>
       </c>
-      <c r="L27" s="24" t="s">
+      <c r="L27" s="21" t="s">
         <v>549</v>
       </c>
-      <c r="M27" s="24" t="s">
+      <c r="M27" s="21" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -3208,14 +3248,14 @@
       <c r="K28" s="11" t="s">
         <v>324</v>
       </c>
-      <c r="L28" s="24" t="s">
+      <c r="L28" s="21" t="s">
         <v>550</v>
       </c>
-      <c r="M28" s="24" t="s">
+      <c r="M28" s="21" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>25</v>
       </c>
@@ -3237,7 +3277,7 @@
       <c r="G29" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="I29" s="21" t="s">
+      <c r="I29" s="18" t="s">
         <v>179</v>
       </c>
       <c r="J29" s="17" t="s">
@@ -3246,14 +3286,14 @@
       <c r="K29" s="17" t="s">
         <v>325</v>
       </c>
-      <c r="L29" s="24" t="s">
+      <c r="L29" s="21" t="s">
         <v>562</v>
       </c>
-      <c r="M29" s="24" t="s">
+      <c r="M29" s="21" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -3282,7 +3322,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -3311,7 +3351,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -3896,10 +3936,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="20">
+      <c r="A1" s="25">
         <v>2010</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="25"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -3917,14 +3957,14 @@
       <c r="D3" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="24" t="s">
         <v>307</v>
       </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="19" t="s">
+      <c r="F3" s="24"/>
+      <c r="G3" s="26" t="s">
         <v>334</v>
       </c>
-      <c r="H3" s="19"/>
+      <c r="H3" s="26"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">

</xml_diff>